<commit_message>
New Object created for every iteration
Boolean result=testData.add(new HashMap<>(dataRecord));
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Price</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Computer</t>
+  </si>
+  <si>
+    <t>Rs. 389</t>
+  </si>
+  <si>
+    <t>Muscle Torque Zip Sweatshirts</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Rs. 1390</t>
   </si>
 </sst>
 </file>
@@ -372,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -402,7 +414,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -418,50 +430,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>